<commit_message>
update hw for lesson 7
</commit_message>
<xml_diff>
--- a/Lesson7/hw_lesson#7_task2.xlsx
+++ b/Lesson7/hw_lesson#7_task2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BI\homeworks\Tamara_Trych\Lesson7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8530D949-2BEB-4BC7-9971-5E82058E40B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A769568-E5D1-44CE-9EB4-E07D3CC417FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12930" yWindow="930" windowWidth="15000" windowHeight="14010" xr2:uid="{83FA2EAA-4B40-4D2A-94F8-69D06506B350}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83FA2EAA-4B40-4D2A-94F8-69D06506B350}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="102">
   <si>
     <t>2НФ</t>
   </si>
@@ -119,9 +119,6 @@
     <t>toyota</t>
   </si>
   <si>
-    <t>speker</t>
-  </si>
-  <si>
     <t>c8</t>
   </si>
   <si>
@@ -342,13 +339,16 @@
   </si>
   <si>
     <t>Отсутствует первичный ключ. Потенциальный первичный ключ - составной: car_id + store, но тогда модель, марка, цвет авто зависил бы от части первичного ключа (от car_id).</t>
+  </si>
+  <si>
+    <t>spyker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,8 +382,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +401,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -501,6 +521,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -528,8 +554,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>422275</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -586,8 +612,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
@@ -647,8 +673,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
@@ -706,7 +732,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
@@ -1166,324 +1192,745 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313251E4-457A-4745-ACF6-447BB77FFD6E}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A24" sqref="A24:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="8" width="11.28515625" customWidth="1"/>
     <col min="11" max="12" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="1">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>11</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="1">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
         <v>37</v>
       </c>
-      <c r="J9" t="s">
+      <c r="F39" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="J39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J40" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K40" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L40" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="J41" s="1">
+        <v>1</v>
+      </c>
+      <c r="K41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="L41" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="1">
-        <v>2</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="J42" s="1">
+        <v>2</v>
+      </c>
+      <c r="K42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L42" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>3</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="1">
+        <v>3</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="1">
-        <v>3</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
         <v>4</v>
       </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C44" s="1">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1">
         <v>4</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F44" s="1">
         <v>4</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J44" s="1">
         <v>4</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L44" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5</v>
+      </c>
+      <c r="J45" s="1">
+        <v>5</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1">
-        <v>5</v>
-      </c>
-      <c r="J15" s="1">
-        <v>5</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
         <v>6</v>
       </c>
-      <c r="C16" s="1">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C46" s="1">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1">
         <v>6</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J46" s="1">
         <v>6</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
         <v>7</v>
       </c>
-      <c r="C17" s="1">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C47" s="1">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1">
         <v>7</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J47" s="1">
         <v>7</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
         <v>8</v>
       </c>
-      <c r="C18" s="1">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C48" s="1">
+        <v>3</v>
+      </c>
+      <c r="D48" s="1">
         <v>8</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J48" s="1">
         <v>8</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K48" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L48" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L18" s="1" t="s">
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1">
+        <v>4</v>
+      </c>
+      <c r="D49" s="1">
+        <v>9</v>
+      </c>
+      <c r="J49" s="1">
+        <v>9</v>
+      </c>
+      <c r="K49" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <v>9</v>
-      </c>
-      <c r="C19" s="1">
-        <v>4</v>
-      </c>
-      <c r="D19" s="1">
-        <v>9</v>
-      </c>
-      <c r="J19" s="1">
-        <v>9</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="1">
+      <c r="L49" s="1">
         <v>626</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
         <v>10</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1">
         <v>10</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J50" s="1">
         <v>10</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
         <v>11</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
         <v>11</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J51" s="1">
         <v>11</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1496,69 +1943,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9152748B-6BAF-4F77-8C98-E9CF776C25FD}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1569,243 +2036,529 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7641D5A2-9FFA-45C9-AB4C-01B3491B3165}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A20" sqref="A20:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="1">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="1">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
         <v>37</v>
       </c>
-      <c r="J9" t="s">
+      <c r="F31" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="J31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K32" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L32" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="L33" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="1">
-        <v>2</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="J34" s="1">
+        <v>2</v>
+      </c>
+      <c r="K34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L34" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="1">
+        <v>3</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="1">
-        <v>3</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
         <v>4</v>
       </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C36" s="1">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1">
         <v>4</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F36" s="1">
         <v>4</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J36" s="1">
         <v>4</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L36" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1">
+        <v>5</v>
+      </c>
+      <c r="J37" s="1">
+        <v>5</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1">
-        <v>5</v>
-      </c>
-      <c r="J15" s="1">
-        <v>5</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
         <v>6</v>
       </c>
-      <c r="C16" s="1">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C38" s="1">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1">
         <v>6</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J38" s="1">
         <v>6</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
         <v>7</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C39" s="1">
         <v>4</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D39" s="1">
         <v>7</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J39" s="1">
         <v>7</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="K39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L39" s="1">
         <v>626</v>
       </c>
     </row>
@@ -1817,26 +2570,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302A2FFB-67CC-4F09-ACDD-A47D1A166EDE}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
     <col min="13" max="13" width="18.140625" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -1849,218 +2605,402 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="3" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="H13" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>203000</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>150</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1118</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>14800</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>10200</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>82399</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>22374</v>
+      </c>
+      <c r="F19" s="1">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="G27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>203000</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="L12" s="6" t="s">
+      <c r="I28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+      <c r="M28" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>203000</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1" t="s">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>150</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I29" s="1">
+        <v>1118</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L29" s="1">
+        <v>2</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>14800</v>
+      </c>
+      <c r="G30" s="1">
+        <v>3</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J30" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>10200</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="1">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>150</v>
-      </c>
-      <c r="G14" s="1">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1118</v>
-      </c>
-      <c r="J14" s="1" t="s">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1">
+        <v>5</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>82399</v>
+      </c>
+      <c r="G32" s="1">
+        <v>5</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="1">
-        <v>2</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>14800</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3</v>
-      </c>
-      <c r="H15" s="1" t="s">
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>22374</v>
+      </c>
+      <c r="G33" s="1">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="I33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1">
-        <v>10200</v>
-      </c>
-      <c r="G16" s="1">
-        <v>4</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>82399</v>
-      </c>
-      <c r="G17" s="1">
-        <v>5</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>22374</v>
-      </c>
-      <c r="G18" s="1">
-        <v>6</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +3037,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2105,15 +3045,15 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
@@ -2122,16 +3062,16 @@
         <v>6</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="8" t="s">
+      <c r="I16" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2139,10 +3079,10 @@
         <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -2151,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
@@ -2162,10 +3102,10 @@
         <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
@@ -2174,7 +3114,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I18" s="1">
         <v>2</v>
@@ -2185,10 +3125,10 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -2197,7 +3137,7 @@
         <v>3</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I19" s="1">
         <v>3</v>
@@ -2208,10 +3148,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="1">
         <v>4</v>
@@ -2220,7 +3160,7 @@
         <v>4</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I20" s="1">
         <v>4</v>
@@ -2228,27 +3168,27 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="G23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="I23" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2256,13 +3196,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="G24" s="1">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="I24" s="1">
         <v>1</v>
@@ -2273,7 +3213,7 @@
         <v>2</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I25" s="1">
         <v>1</v>
@@ -2284,7 +3224,7 @@
         <v>3</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
@@ -2295,7 +3235,7 @@
         <v>4</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I27" s="1">
         <v>1</v>
@@ -2309,10 +3249,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9194129D-4EA2-4F45-A251-D7CF660BF6E5}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,68 +3264,128 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="C15" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>23</v>
-      </c>
-      <c r="C15" s="1">
-        <v>13.44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1">
+        <v>13.44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>24</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C17" s="1">
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
         <v>25</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="1">
         <v>543.44000000000005</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
         <v>19</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C19" s="11">
         <v>34.5</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1">
+        <v>13.44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1">
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1">
+        <v>543.44000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>19</v>
+      </c>
+      <c r="D27" s="11">
+        <v>34.5</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>